<commit_message>
build initial rails resources based on design
</commit_message>
<xml_diff>
--- a/Database Schema - Stock App.xlsx
+++ b/Database Schema - Stock App.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acapp5K1/Desktop/stocks-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E35B962F-9961-5C47-9036-7015D3E75BCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A4A324C-89A7-4748-A4F0-A24FE7E06785}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="0" windowWidth="25600" windowHeight="28800" xr2:uid="{4C8372E1-6D7C-B64A-8DDC-56B8C8C6FD40}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="77">
   <si>
     <t>COLUMN</t>
   </si>
@@ -95,15 +95,6 @@
     <t>companies</t>
   </si>
   <si>
-    <t>symbols</t>
-  </si>
-  <si>
-    <t>symbol</t>
-  </si>
-  <si>
-    <t>security_name</t>
-  </si>
-  <si>
     <t>watchlists</t>
   </si>
   <si>
@@ -128,12 +119,6 @@
     <t>watchlists_companies</t>
   </si>
   <si>
-    <t>has_many :companies, through: watchlists_companies</t>
-  </si>
-  <si>
-    <t>has_many :watchlists_companies</t>
-  </si>
-  <si>
     <t>belongs_to :watchlist</t>
   </si>
   <si>
@@ -176,28 +161,109 @@
     <t>52_week_low_date</t>
   </si>
   <si>
-    <t>has_many :watchlists, through: watchlists_companies</t>
-  </si>
-  <si>
     <t>float</t>
   </si>
   <si>
-    <t>has_one :company</t>
-  </si>
-  <si>
     <t>company_id</t>
   </si>
   <si>
     <t>charts</t>
   </si>
   <si>
-    <t>has_one :chart</t>
-  </si>
-  <si>
-    <t>chart_data</t>
-  </si>
-  <si>
-    <t>array / string?</t>
+    <t>Future in Green</t>
+  </si>
+  <si>
+    <t>Charts:</t>
+  </si>
+  <si>
+    <t>Data from API:</t>
+  </si>
+  <si>
+    <t>Data needed for chart:</t>
+  </si>
+  <si>
+    <t>chart.data = [ {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "date": "2011-08-01",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "open": "136.65",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "high": "136.96",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "low": "134.15",</t>
+  </si>
+  <si>
+    <t>{c:[321.85, 323.24, …],</t>
+  </si>
+  <si>
+    <t>{h: [array…],</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "close": "136.49"},…]</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>close</t>
+  </si>
+  <si>
+    <t>companies_charts</t>
+  </si>
+  <si>
+    <t>chart_type</t>
+  </si>
+  <si>
+    <t>['candle', 'xy', etc]</t>
+  </si>
+  <si>
+    <t>chart_id</t>
+  </si>
+  <si>
+    <t>ticker</t>
+  </si>
+  <si>
+    <t>tickers</t>
+  </si>
+  <si>
+    <t>ticker_name</t>
+  </si>
+  <si>
+    <t>belongs_to :chart</t>
+  </si>
+  <si>
+    <t>has_many :watchlist_companies</t>
+  </si>
+  <si>
+    <t>has_many :companies, through: :watchlist_companies</t>
+  </si>
+  <si>
+    <t>has_many :watchlists, through: :watchlist_companies</t>
+  </si>
+  <si>
+    <t>has_many :company_charts</t>
+  </si>
+  <si>
+    <t>has_many :charts, through: :company_charts</t>
+  </si>
+  <si>
+    <t>has_many :companies, through: :company_charts</t>
   </si>
 </sst>
 </file>
@@ -221,12 +287,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -327,17 +399,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -352,6 +415,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -666,10 +741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6B6C358-AFD7-4C46-89BD-F9EA1474856F}">
-  <dimension ref="B2:D91"/>
+  <dimension ref="B2:D121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B108" sqref="B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -683,594 +758,759 @@
       <c r="B2" t="s">
         <v>8</v>
       </c>
+      <c r="D2" s="13" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="3" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="3"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="11"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="8"/>
+      <c r="D6" s="5"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="8"/>
+      <c r="D7" s="5"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="8"/>
+      <c r="C8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="14"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="8"/>
+      <c r="C9" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="14"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="8"/>
+      <c r="C10" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="14"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="8"/>
+      <c r="C11" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="14"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="8"/>
+      <c r="D12" s="5"/>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="8"/>
+      <c r="D13" s="5"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="8"/>
+      <c r="C14" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="14"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="8" t="s">
+      <c r="C15" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="14" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B16" s="7"/>
-      <c r="D16" s="8"/>
+      <c r="B16" s="4"/>
+      <c r="D16" s="5"/>
     </row>
     <row r="17" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="9"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="11"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="8"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="3"/>
+      <c r="B22" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="10"/>
+      <c r="D22" s="11"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="8"/>
+      <c r="D24" s="5"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="7" t="s">
-        <v>21</v>
+      <c r="B25" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="C25" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="8"/>
+      <c r="D25" s="5"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B26" s="7" t="s">
-        <v>22</v>
+      <c r="B26" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="C26" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="8"/>
+      <c r="D26" s="5"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="7"/>
-      <c r="D27" s="8"/>
+      <c r="B27" s="4"/>
+      <c r="D27" s="5"/>
     </row>
     <row r="28" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="9"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="11"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="8"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B33" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="3"/>
+      <c r="B33" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="10"/>
+      <c r="D33" s="11"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
       </c>
-      <c r="D35" s="8"/>
+      <c r="D35" s="5"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C36" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="8"/>
+      <c r="D36" s="5"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C37" t="s">
         <v>6</v>
       </c>
-      <c r="D37" s="8"/>
+      <c r="D37" s="5"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B38" s="7" t="s">
-        <v>24</v>
+      <c r="B38" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="C38" t="s">
-        <v>25</v>
-      </c>
-      <c r="D38" s="8"/>
+        <v>22</v>
+      </c>
+      <c r="D38" s="5"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B39" s="7"/>
-      <c r="D39" s="8"/>
+      <c r="B39" s="4"/>
+      <c r="D39" s="5"/>
     </row>
     <row r="40" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="9"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="11"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="8"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="46" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B46" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C46" s="2"/>
-      <c r="D46" s="3"/>
+      <c r="B46" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C46" s="10"/>
+      <c r="D46" s="11"/>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="D47" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C48" t="s">
         <v>4</v>
       </c>
-      <c r="D48" s="8"/>
+      <c r="D48" s="5"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B49" s="7" t="s">
-        <v>26</v>
+      <c r="B49" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="C49" t="s">
-        <v>25</v>
-      </c>
-      <c r="D49" s="8"/>
+        <v>22</v>
+      </c>
+      <c r="D49" s="5"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B50" s="7" t="s">
-        <v>50</v>
+      <c r="B50" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="C50" t="s">
-        <v>25</v>
-      </c>
-      <c r="D50" s="8"/>
+        <v>22</v>
+      </c>
+      <c r="D50" s="5"/>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B51" s="7"/>
-      <c r="D51" s="8"/>
+      <c r="B51" s="4"/>
+      <c r="D51" s="5"/>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B52" s="7"/>
-      <c r="D52" s="8"/>
+      <c r="B52" s="4"/>
+      <c r="D52" s="5"/>
     </row>
     <row r="53" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="9"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="11"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="8"/>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="58" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="59" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B59" s="1" t="s">
+      <c r="B59" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C59" s="2"/>
-      <c r="D59" s="3"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="11"/>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="C60" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D60" s="6" t="s">
+      <c r="D60" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B61" s="7" t="s">
+      <c r="B61" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C61" t="s">
         <v>4</v>
       </c>
-      <c r="D61" s="8"/>
+      <c r="D61" s="5"/>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B62" s="7" t="s">
-        <v>21</v>
+      <c r="B62" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="C62" t="s">
         <v>6</v>
       </c>
-      <c r="D62" s="8"/>
+      <c r="D62" s="5"/>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B63" s="7" t="s">
+      <c r="B63" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C63" t="s">
         <v>6</v>
       </c>
-      <c r="D63" s="8"/>
+      <c r="D63" s="5"/>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B64" s="7" t="s">
+      <c r="B64" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C64" t="s">
+        <v>6</v>
+      </c>
+      <c r="D64" s="5"/>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B65" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C65" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" s="5"/>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B66" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C66" t="s">
+        <v>42</v>
+      </c>
+      <c r="D66" s="5"/>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B67" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C67" t="s">
+        <v>42</v>
+      </c>
+      <c r="D67" s="5"/>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B68" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C68" t="s">
+        <v>6</v>
+      </c>
+      <c r="D68" s="5"/>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B69" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C64" t="s">
-        <v>6</v>
-      </c>
-      <c r="D64" s="8"/>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B65" s="7" t="s">
+      <c r="C69" t="s">
+        <v>6</v>
+      </c>
+      <c r="D69" s="5"/>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B70" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C65" t="s">
-        <v>6</v>
-      </c>
-      <c r="D65" s="8"/>
-    </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B66" s="7" t="s">
+      <c r="C70" t="s">
+        <v>6</v>
+      </c>
+      <c r="D70" s="5"/>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B71" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C66" t="s">
-        <v>48</v>
-      </c>
-      <c r="D66" s="8"/>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B67" s="7" t="s">
+      <c r="C71" t="s">
+        <v>42</v>
+      </c>
+      <c r="D71" s="5"/>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B72" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C67" t="s">
-        <v>48</v>
-      </c>
-      <c r="D67" s="8"/>
-    </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B68" s="7" t="s">
+      <c r="C72" t="s">
+        <v>42</v>
+      </c>
+      <c r="D72" s="5"/>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B73" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C68" t="s">
-        <v>6</v>
-      </c>
-      <c r="D68" s="8"/>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B69" s="7" t="s">
+      <c r="C73" t="s">
+        <v>42</v>
+      </c>
+      <c r="D73" s="5"/>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B74" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C69" t="s">
-        <v>6</v>
-      </c>
-      <c r="D69" s="8"/>
-    </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B70" s="7" t="s">
+      <c r="C74" t="s">
+        <v>42</v>
+      </c>
+      <c r="D74" s="5"/>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B75" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C70" t="s">
-        <v>6</v>
-      </c>
-      <c r="D70" s="8"/>
-    </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B71" s="7" t="s">
+      <c r="C75" t="s">
         <v>42</v>
       </c>
-      <c r="C71" t="s">
-        <v>48</v>
-      </c>
-      <c r="D71" s="8"/>
-    </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B72" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C72" t="s">
-        <v>48</v>
-      </c>
-      <c r="D72" s="8"/>
-    </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B73" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C73" t="s">
-        <v>48</v>
-      </c>
-      <c r="D73" s="8"/>
-    </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B74" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C74" t="s">
-        <v>48</v>
-      </c>
-      <c r="D74" s="8"/>
-    </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B75" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C75" t="s">
-        <v>48</v>
-      </c>
-      <c r="D75" s="8"/>
+      <c r="D75" s="5"/>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B76" s="7"/>
-      <c r="D76" s="8"/>
+      <c r="B76" s="4"/>
+      <c r="D76" s="5"/>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B77" s="7"/>
-      <c r="D77" s="8"/>
+      <c r="B77" s="4"/>
+      <c r="D77" s="5"/>
     </row>
     <row r="78" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="9"/>
-      <c r="C78" s="10"/>
-      <c r="D78" s="11"/>
+      <c r="B78" s="6"/>
+      <c r="C78" s="7"/>
+      <c r="D78" s="8"/>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B82" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B85" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C85" s="10"/>
+      <c r="D85" s="11"/>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B87" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C87" t="s">
+        <v>4</v>
+      </c>
+      <c r="D87" s="5"/>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B88" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C88" t="s">
+        <v>22</v>
+      </c>
+      <c r="D88" s="5"/>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B89" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C89" t="s">
+        <v>22</v>
+      </c>
+      <c r="D89" s="5"/>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B90" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C90" t="s">
+        <v>6</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B91" s="4"/>
+      <c r="D91" s="5"/>
+    </row>
+    <row r="92" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B92" s="6"/>
+      <c r="C92" s="7"/>
+      <c r="D92" s="8"/>
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B93" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B94" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B97" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C97" s="10"/>
+      <c r="D97" s="11"/>
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B98" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B99" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C99" t="s">
+        <v>4</v>
+      </c>
+      <c r="D99" s="5"/>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B100" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C100" t="s">
+        <v>6</v>
+      </c>
+      <c r="D100" s="5"/>
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B101" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C101" t="s">
+        <v>6</v>
+      </c>
+      <c r="D101" s="5"/>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B102" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C102" t="s">
+        <v>6</v>
+      </c>
+      <c r="D102" s="5"/>
+    </row>
+    <row r="103" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B103" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C103" t="s">
+        <v>6</v>
+      </c>
+      <c r="D103" s="5"/>
+    </row>
+    <row r="104" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B104" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C104" t="s">
+        <v>6</v>
+      </c>
+      <c r="D104" s="5"/>
+    </row>
+    <row r="105" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B105" s="6"/>
+      <c r="C105" s="7"/>
+      <c r="D105" s="8"/>
+    </row>
+    <row r="106" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B106" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="107" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B107" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B110" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B111" t="s">
+        <v>47</v>
+      </c>
+      <c r="C111" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="112" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C112" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C113" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="116" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B116" t="s">
+        <v>48</v>
+      </c>
+      <c r="C116" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C117" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C118" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="119" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C119" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="82" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B83" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C83" s="2"/>
-      <c r="D83" s="3"/>
-    </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B84" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C84" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D84" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B85" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C85" t="s">
-        <v>4</v>
-      </c>
-      <c r="D85" s="8"/>
-    </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B86" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C86" t="s">
-        <v>25</v>
-      </c>
-      <c r="D86" s="8"/>
-    </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B87" s="7" t="s">
+    <row r="120" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C120" t="s">
         <v>53</v>
       </c>
-      <c r="C87" t="s">
-        <v>54</v>
-      </c>
-      <c r="D87" s="8"/>
-    </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B88" s="7"/>
-      <c r="D88" s="8"/>
-    </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B89" s="7"/>
-      <c r="D89" s="8"/>
-    </row>
-    <row r="90" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="9"/>
-      <c r="C90" s="10"/>
-      <c r="D90" s="11"/>
-    </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B91" t="s">
-        <v>49</v>
+    </row>
+    <row r="121" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C121" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="B97:D97"/>
+    <mergeCell ref="B85:D85"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B33:D33"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B46:D46"/>
     <mergeCell ref="B59:D59"/>
-    <mergeCell ref="B83:D83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
persist chart data to database add serializers
</commit_message>
<xml_diff>
--- a/Database Schema - Stock App.xlsx
+++ b/Database Schema - Stock App.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acapp5K1/Desktop/stocks-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4582A010-675E-0C49-BDDC-CBD28C3E2964}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE0D631-8079-3949-B939-2B88F538B6C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="0" windowWidth="25600" windowHeight="28800" xr2:uid="{4C8372E1-6D7C-B64A-8DDC-56B8C8C6FD40}"/>
+    <workbookView xWindow="-19200" yWindow="0" windowWidth="19200" windowHeight="21600" xr2:uid="{4C8372E1-6D7C-B64A-8DDC-56B8C8C6FD40}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="76">
   <si>
     <t>COLUMN</t>
   </si>
@@ -251,19 +251,16 @@
     <t>has_many :watchlists, through: :watchlist_companies</t>
   </si>
   <si>
-    <t>has_many :company_charts</t>
-  </si>
-  <si>
-    <t>has_many :charts, through: :company_charts</t>
-  </si>
-  <si>
-    <t>has_many :companies, through: :company_charts</t>
-  </si>
-  <si>
     <t>watchlist_companies</t>
   </si>
   <si>
-    <t>company_charts</t>
+    <t>has_many :charts</t>
+  </si>
+  <si>
+    <t>chart_lines</t>
+  </si>
+  <si>
+    <t>has_many :chart_lines</t>
   </si>
 </sst>
 </file>
@@ -415,6 +412,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -424,9 +424,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -743,8 +740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6B6C358-AFD7-4C46-89BD-F9EA1474856F}">
   <dimension ref="B2:D121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -758,17 +755,17 @@
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="10" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="14"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
@@ -800,40 +797,40 @@
       <c r="D7" s="5"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="14"/>
+      <c r="C8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="11"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="14"/>
+      <c r="C9" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="11"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="14"/>
+      <c r="C10" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="11"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="14"/>
+      <c r="C11" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="11"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="s">
@@ -854,22 +851,22 @@
       <c r="D13" s="5"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="14"/>
+      <c r="C14" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="11"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="14" t="s">
+      <c r="C15" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>18</v>
       </c>
     </row>
@@ -889,11 +886,11 @@
     </row>
     <row r="21" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="11"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="14"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
@@ -954,11 +951,11 @@
     </row>
     <row r="32" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="10"/>
-      <c r="D33" s="11"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="14"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
@@ -1033,11 +1030,11 @@
     </row>
     <row r="45" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="46" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B46" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="C46" s="10"/>
-      <c r="D46" s="11"/>
+      <c r="B46" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C46" s="13"/>
+      <c r="D46" s="14"/>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
@@ -1102,11 +1099,11 @@
     </row>
     <row r="58" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="59" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B59" s="9" t="s">
+      <c r="B59" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C59" s="10"/>
-      <c r="D59" s="11"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="14"/>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B60" s="1" t="s">
@@ -1279,21 +1276,16 @@
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B82" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="84" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="85" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B85" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C85" s="10"/>
-      <c r="D85" s="11"/>
+      <c r="B85" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C85" s="13"/>
+      <c r="D85" s="14"/>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B86" s="1" t="s">
@@ -1326,68 +1318,68 @@
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B89" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C89" t="s">
-        <v>22</v>
-      </c>
-      <c r="D89" s="5"/>
+        <v>6</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B90" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C90" t="s">
-        <v>6</v>
-      </c>
-      <c r="D90" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B91" s="4"/>
-      <c r="D91" s="5"/>
-    </row>
-    <row r="92" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B92" s="6"/>
-      <c r="C92" s="7"/>
-      <c r="D92" s="8"/>
+      <c r="B90" s="4"/>
+      <c r="D90" s="5"/>
+    </row>
+    <row r="91" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B91" s="6"/>
+      <c r="C91" s="7"/>
+      <c r="D91" s="8"/>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B92" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B94" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="96" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="96" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B96" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C96" s="13"/>
+      <c r="D96" s="14"/>
+    </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B97" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C97" s="10"/>
-      <c r="D97" s="11"/>
+      <c r="B97" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B98" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D98" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="B98" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C98" t="s">
+        <v>4</v>
+      </c>
+      <c r="D98" s="5"/>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B99" s="4" t="s">
-        <v>3</v>
+        <v>64</v>
       </c>
       <c r="C99" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D99" s="5"/>
     </row>
@@ -1443,12 +1435,7 @@
     </row>
     <row r="106" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B107" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="110" spans="2:4" x14ac:dyDescent="0.2">
@@ -1509,7 +1496,7 @@
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B97:D97"/>
+    <mergeCell ref="B96:D96"/>
     <mergeCell ref="B85:D85"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B33:D33"/>

</xml_diff>

<commit_message>
add current stock price to company data
</commit_message>
<xml_diff>
--- a/Database Schema - Stock App.xlsx
+++ b/Database Schema - Stock App.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acapp5K1/Desktop/stocks-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE0D631-8079-3949-B939-2B88F538B6C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AFA0E43-41FF-FE4C-A5AD-217CD17FCAD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19200" yWindow="0" windowWidth="19200" windowHeight="21600" xr2:uid="{4C8372E1-6D7C-B64A-8DDC-56B8C8C6FD40}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="78">
   <si>
     <t>COLUMN</t>
   </si>
@@ -261,6 +261,12 @@
   </si>
   <si>
     <t>has_many :chart_lines</t>
+  </si>
+  <si>
+    <t>current_price</t>
+  </si>
+  <si>
+    <t>previous_close_price</t>
   </si>
 </sst>
 </file>
@@ -738,10 +744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6B6C358-AFD7-4C46-89BD-F9EA1474856F}">
-  <dimension ref="B2:D121"/>
+  <dimension ref="B2:D123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1208,25 +1214,25 @@
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B71" s="4" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="C71" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="D71" s="5"/>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B72" s="4" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="C72" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="D72" s="5"/>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B73" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C73" t="s">
         <v>41</v>
@@ -1235,7 +1241,7 @@
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B74" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C74" t="s">
         <v>41</v>
@@ -1244,7 +1250,7 @@
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B75" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C75" t="s">
         <v>41</v>
@@ -1252,158 +1258,158 @@
       <c r="D75" s="5"/>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B76" s="4"/>
+      <c r="B76" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C76" t="s">
+        <v>41</v>
+      </c>
       <c r="D76" s="5"/>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B77" s="4"/>
+      <c r="B77" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C77" t="s">
+        <v>41</v>
+      </c>
       <c r="D77" s="5"/>
     </row>
-    <row r="78" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="6"/>
-      <c r="C78" s="7"/>
-      <c r="D78" s="8"/>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B78" s="4"/>
+      <c r="D78" s="5"/>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B79" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B80" t="s">
-        <v>71</v>
-      </c>
+      <c r="B79" s="4"/>
+      <c r="D79" s="5"/>
+    </row>
+    <row r="80" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B80" s="6"/>
+      <c r="C80" s="7"/>
+      <c r="D80" s="8"/>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B82" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B83" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="84" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B85" s="12" t="s">
+    <row r="86" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B87" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C85" s="13"/>
-      <c r="D85" s="14"/>
-    </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B86" s="1" t="s">
+      <c r="C87" s="13"/>
+      <c r="D87" s="14"/>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B88" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C86" s="2" t="s">
+      <c r="C88" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D86" s="3" t="s">
+      <c r="D88" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B87" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C87" t="s">
-        <v>4</v>
-      </c>
-      <c r="D87" s="5"/>
-    </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B88" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C88" t="s">
-        <v>22</v>
-      </c>
-      <c r="D88" s="5"/>
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B89" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C89" t="s">
+        <v>4</v>
+      </c>
+      <c r="D89" s="5"/>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B90" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C90" t="s">
+        <v>22</v>
+      </c>
+      <c r="D90" s="5"/>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B91" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C89" t="s">
-        <v>6</v>
-      </c>
-      <c r="D89" s="5" t="s">
+      <c r="C91" t="s">
+        <v>6</v>
+      </c>
+      <c r="D91" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B90" s="4"/>
-      <c r="D90" s="5"/>
-    </row>
-    <row r="91" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="6"/>
-      <c r="C91" s="7"/>
-      <c r="D91" s="8"/>
-    </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B92" t="s">
+      <c r="B92" s="4"/>
+      <c r="D92" s="5"/>
+    </row>
+    <row r="93" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B93" s="6"/>
+      <c r="C93" s="7"/>
+      <c r="D93" s="8"/>
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B94" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B93" t="s">
+    <row r="95" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B95" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="95" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="96" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B96" s="12" t="s">
+    <row r="97" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B98" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C96" s="13"/>
-      <c r="D96" s="14"/>
-    </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B97" s="1" t="s">
+      <c r="C98" s="13"/>
+      <c r="D98" s="14"/>
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B99" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C97" s="2" t="s">
+      <c r="C99" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D97" s="3" t="s">
+      <c r="D99" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B98" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C98" t="s">
-        <v>4</v>
-      </c>
-      <c r="D98" s="5"/>
-    </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B99" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C99" t="s">
-        <v>22</v>
-      </c>
-      <c r="D99" s="5"/>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B100" s="4" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="C100" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D100" s="5"/>
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B101" s="4" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C101" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D101" s="5"/>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B102" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C102" t="s">
         <v>6</v>
@@ -1412,7 +1418,7 @@
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B103" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C103" t="s">
         <v>6</v>
@@ -1421,83 +1427,101 @@
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B104" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C104" t="s">
+        <v>6</v>
+      </c>
+      <c r="D104" s="5"/>
+    </row>
+    <row r="105" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B105" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C105" t="s">
+        <v>6</v>
+      </c>
+      <c r="D105" s="5"/>
+    </row>
+    <row r="106" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B106" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C104" t="s">
-        <v>6</v>
-      </c>
-      <c r="D104" s="5"/>
-    </row>
-    <row r="105" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B105" s="6"/>
-      <c r="C105" s="7"/>
-      <c r="D105" s="8"/>
-    </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B106" t="s">
+      <c r="C106" t="s">
+        <v>6</v>
+      </c>
+      <c r="D106" s="5"/>
+    </row>
+    <row r="107" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B107" s="6"/>
+      <c r="C107" s="7"/>
+      <c r="D107" s="8"/>
+    </row>
+    <row r="108" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B108" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="110" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B110" t="s">
+    <row r="112" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B112" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B111" t="s">
+    <row r="113" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B113" t="s">
         <v>46</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C113" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C112" t="s">
+    <row r="114" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C114" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C113" t="s">
+    <row r="115" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C115" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B116" t="s">
+    <row r="118" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B118" t="s">
         <v>47</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C118" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C117" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C118" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C119" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C120" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C121" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="122" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C122" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="123" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C123" t="s">
         <v>59</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B96:D96"/>
-    <mergeCell ref="B85:D85"/>
+    <mergeCell ref="B98:D98"/>
+    <mergeCell ref="B87:D87"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B33:D33"/>
     <mergeCell ref="B4:D4"/>

</xml_diff>

<commit_message>
update rails to accept chart date range
</commit_message>
<xml_diff>
--- a/Database Schema - Stock App.xlsx
+++ b/Database Schema - Stock App.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acapp5K1/Desktop/stocks-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AFA0E43-41FF-FE4C-A5AD-217CD17FCAD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495649B0-22CA-9446-AB79-A9ABB5ABFF33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19200" yWindow="0" windowWidth="19200" windowHeight="21600" xr2:uid="{4C8372E1-6D7C-B64A-8DDC-56B8C8C6FD40}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="80">
   <si>
     <t>COLUMN</t>
   </si>
@@ -267,6 +267,12 @@
   </si>
   <si>
     <t>previous_close_price</t>
+  </si>
+  <si>
+    <t>start_date</t>
+  </si>
+  <si>
+    <t>end_date</t>
   </si>
 </sst>
 </file>
@@ -744,10 +750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6B6C358-AFD7-4C46-89BD-F9EA1474856F}">
-  <dimension ref="B2:D123"/>
+  <dimension ref="B2:D125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="C93" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1342,92 +1348,92 @@
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B91" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C91" t="s">
+        <v>6</v>
+      </c>
+      <c r="D91" s="5"/>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B92" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C92" t="s">
+        <v>6</v>
+      </c>
+      <c r="D92" s="5"/>
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B93" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C91" t="s">
-        <v>6</v>
-      </c>
-      <c r="D91" s="5" t="s">
+      <c r="C93" t="s">
+        <v>6</v>
+      </c>
+      <c r="D93" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B92" s="4"/>
-      <c r="D92" s="5"/>
-    </row>
-    <row r="93" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="6"/>
-      <c r="C93" s="7"/>
-      <c r="D93" s="8"/>
-    </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B94" t="s">
+      <c r="B94" s="4"/>
+      <c r="D94" s="5"/>
+    </row>
+    <row r="95" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B95" s="6"/>
+      <c r="C95" s="7"/>
+      <c r="D95" s="8"/>
+    </row>
+    <row r="96" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B96" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="95" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B95" t="s">
+    <row r="97" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B97" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="97" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B98" s="12" t="s">
+    <row r="99" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B100" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C98" s="13"/>
-      <c r="D98" s="14"/>
-    </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B99" s="1" t="s">
+      <c r="C100" s="13"/>
+      <c r="D100" s="14"/>
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B101" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C99" s="2" t="s">
+      <c r="C101" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D99" s="3" t="s">
+      <c r="D101" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B100" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C100" t="s">
-        <v>4</v>
-      </c>
-      <c r="D100" s="5"/>
-    </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B101" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C101" t="s">
-        <v>22</v>
-      </c>
-      <c r="D101" s="5"/>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B102" s="4" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="C102" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D102" s="5"/>
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B103" s="4" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C103" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D103" s="5"/>
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B104" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C104" t="s">
         <v>6</v>
@@ -1436,7 +1442,7 @@
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B105" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C105" t="s">
         <v>6</v>
@@ -1445,82 +1451,100 @@
     </row>
     <row r="106" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B106" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C106" t="s">
+        <v>6</v>
+      </c>
+      <c r="D106" s="5"/>
+    </row>
+    <row r="107" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B107" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C107" t="s">
+        <v>6</v>
+      </c>
+      <c r="D107" s="5"/>
+    </row>
+    <row r="108" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B108" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C106" t="s">
-        <v>6</v>
-      </c>
-      <c r="D106" s="5"/>
-    </row>
-    <row r="107" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B107" s="6"/>
-      <c r="C107" s="7"/>
-      <c r="D107" s="8"/>
-    </row>
-    <row r="108" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B108" t="s">
+      <c r="C108" t="s">
+        <v>6</v>
+      </c>
+      <c r="D108" s="5"/>
+    </row>
+    <row r="109" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B109" s="6"/>
+      <c r="C109" s="7"/>
+      <c r="D109" s="8"/>
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B110" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B112" t="s">
+    <row r="114" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B114" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B113" t="s">
+    <row r="115" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B115" t="s">
         <v>46</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C115" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C114" t="s">
+    <row r="116" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C116" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C115" t="s">
+    <row r="117" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C117" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B118" t="s">
+    <row r="120" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B120" t="s">
         <v>47</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C120" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C119" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C120" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C121" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C122" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="123" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C123" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="124" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C124" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="125" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C125" t="s">
         <v>59</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B98:D98"/>
+    <mergeCell ref="B100:D100"/>
     <mergeCell ref="B87:D87"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B33:D33"/>

</xml_diff>